<commit_message>
incorporated changes to handle testng parameters
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/data.xlsx
+++ b/src/test/resources/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyLearning\SeleniumFramework\luma_alt\ecommerce\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9B97FD-9D32-4D63-AEE9-F942369049B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED1B36C-4F1C-4F06-89AD-BAEFCFF513E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B0959001-371E-481F-BFDB-AB5BDA66A140}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>FirstName</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>fl28@test.com</t>
+  </si>
+  <si>
+    <t>firstName40</t>
+  </si>
+  <si>
+    <t>lastName40</t>
+  </si>
+  <si>
+    <t>fl40@test.com</t>
   </si>
 </sst>
 </file>
@@ -470,7 +479,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,13 +506,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>

</xml_diff>